<commit_message>
ARREGLOS DE CAPTCHA BOT
</commit_message>
<xml_diff>
--- a/citas/ALAJUELA_citas_disponibles.xlsx
+++ b/citas/ALAJUELA_citas_disponibles.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Martes 14/05/2024</t>
+          <t>Miércoles 15/05/2024</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Miércoles 15/05/2024</t>
+          <t>Lunes 20/05/2024</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lunes 20/05/2024</t>
+          <t>Martes 21/05/2024</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Martes 21/05/2024</t>
+          <t>Miércoles 22/05/2024</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Miércoles 22/05/2024</t>
+          <t>Lunes 27/05/2024</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lunes 27/05/2024</t>
+          <t>Martes 28/05/2024</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Martes 28/05/2024</t>
+          <t>Miércoles 29/05/2024</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miércoles 29/05/2024</t>
+          <t>Lunes 03/06/2024</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lunes 03/06/2024</t>
+          <t>Martes 04/06/2024</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Martes 04/06/2024</t>
+          <t>Miércoles 05/06/2024</t>
         </is>
       </c>
     </row>

</xml_diff>